<commit_message>
ADD nav bar - logout btn
</commit_message>
<xml_diff>
--- a/DB/engine.xlsx
+++ b/DB/engine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkhh\PycharmProjects\flaskProject\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박동환\PycharmProjects\InventoryManagement\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F274E2B-6521-4309-B2BE-16C545FEB2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9CBD3F-8087-41D0-9154-0B75AB33DC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="2970" windowWidth="21600" windowHeight="10695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3705" yWindow="1305" windowWidth="18135" windowHeight="13365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="engineDB" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="218">
   <si>
     <t>eid</t>
   </si>
@@ -671,6 +671,14 @@
   </si>
   <si>
     <t>qw</t>
+  </si>
+  <si>
+    <t>BE01</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>베타</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -867,7 +875,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -913,6 +921,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1224,10 +1233,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
@@ -1471,6 +1480,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>259753</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="5">
+        <v>20220809</v>
+      </c>
+      <c r="E10" s="5">
+        <v>20220810</v>
+      </c>
+      <c r="H10" s="5">
+        <v>10003</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092901" footer="0.30000001192092901"/>
@@ -1481,10 +1513,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
@@ -1503,6 +1535,11 @@
     <row r="2" spans="1:2">
       <c r="A2" s="5">
         <v>10002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="5">
+        <v>10003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD nav bar - a tag, logout btn, ...
</commit_message>
<xml_diff>
--- a/DB/engine.xlsx
+++ b/DB/engine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박동환\PycharmProjects\InventoryManagement\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkhh\PycharmProjects\flaskProject\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9CBD3F-8087-41D0-9154-0B75AB33DC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F274E2B-6521-4309-B2BE-16C545FEB2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="1305" windowWidth="18135" windowHeight="13365" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4050" yWindow="2970" windowWidth="21600" windowHeight="10695" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="engineDB" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="216">
   <si>
     <t>eid</t>
   </si>
@@ -671,14 +671,6 @@
   </si>
   <si>
     <t>qw</t>
-  </si>
-  <si>
-    <t>BE01</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>베타</t>
-    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -875,7 +867,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -921,7 +913,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1233,10 +1224,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
@@ -1480,29 +1471,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="A10">
-        <v>259753</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>217</v>
-      </c>
-      <c r="D10" s="5">
-        <v>20220809</v>
-      </c>
-      <c r="E10" s="5">
-        <v>20220810</v>
-      </c>
-      <c r="H10" s="5">
-        <v>10003</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092901" footer="0.30000001192092901"/>
@@ -1513,10 +1481,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5"/>
@@ -1535,11 +1503,6 @@
     <row r="2" spans="1:2">
       <c r="A2" s="5">
         <v>10002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5">
-        <v>10003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>